<commit_message>
explicit separation of boundaries between regions & boundaries between subregions for easier code maintenance
</commit_message>
<xml_diff>
--- a/src/documentation/references/IteratorVariableData/Region3/IAPWS-IF97-Region3-VPT.xlsx
+++ b/src/documentation/references/IteratorVariableData/Region3/IAPWS-IF97-Region3-VPT.xlsx
@@ -1,18 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyData\GithubRepos\Active\WaterThermodynamicProperties\src\documentation\references\IteratorVariableData\Region3\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46248BE8-31A1-4116-B0F4-68734247E4DA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11655"/>
+    <workbookView xWindow="14364" yWindow="8076" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -2919,8 +2931,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2980,7 +2992,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3250,56 +3262,57 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AR184"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:AS184"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="A129" sqref="A129"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="23" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="23" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="23" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="43" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="9.140625" customWidth="1"/>
-    <col min="46" max="16384" width="9.140625" hidden="1"/>
+    <col min="26" max="27" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="43" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="9.109375" customWidth="1"/>
+    <col min="46" max="16384" width="9.109375" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="1" customFormat="1">
+    <row r="1" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
@@ -3310,12 +3323,12 @@
         <v>963</v>
       </c>
     </row>
-    <row r="3" spans="1:33" s="3" customFormat="1">
+    <row r="3" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>916</v>
       </c>
@@ -3335,7 +3348,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>914</v>
       </c>
@@ -3355,12 +3368,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:33" s="3" customFormat="1">
+    <row r="6" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:33">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>916</v>
       </c>
@@ -3455,7 +3468,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:33">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>915</v>
       </c>
@@ -3550,7 +3563,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:33">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>914</v>
       </c>
@@ -3645,13 +3658,13 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:33"/>
-    <row r="11" spans="1:33" s="3" customFormat="1">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:33">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>914</v>
       </c>
@@ -3665,13 +3678,13 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:33"/>
-    <row r="14" spans="1:33" s="3" customFormat="1">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:33">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>916</v>
       </c>
@@ -3772,7 +3785,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:33">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>915</v>
       </c>
@@ -3873,7 +3886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:39">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>914</v>
       </c>
@@ -3974,13 +3987,13 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:39"/>
-    <row r="19" spans="1:39" s="3" customFormat="1">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:39" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:39">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>914</v>
       </c>
@@ -4015,13 +4028,13 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:39"/>
-    <row r="22" spans="1:39" s="3" customFormat="1">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:39" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:39">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>916</v>
       </c>
@@ -4038,7 +4051,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:39">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>914</v>
       </c>
@@ -4055,13 +4068,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:39"/>
-    <row r="26" spans="1:39" s="3" customFormat="1">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:39" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:39">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>916</v>
       </c>
@@ -4171,7 +4184,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:39">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>915</v>
       </c>
@@ -4281,7 +4294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:39">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>914</v>
       </c>
@@ -4391,13 +4404,13 @@
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="1:39"/>
-    <row r="31" spans="1:39" s="3" customFormat="1">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:39" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="32" spans="1:39">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>916</v>
       </c>
@@ -4516,7 +4529,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:43">
+    <row r="33" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>915</v>
       </c>
@@ -4635,7 +4648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:43">
+    <row r="34" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>914</v>
       </c>
@@ -4754,13 +4767,13 @@
         <v>164</v>
       </c>
     </row>
-    <row r="35" spans="1:43"/>
-    <row r="36" spans="1:43" s="3" customFormat="1">
+    <row r="35" spans="1:43" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="37" spans="1:43">
+    <row r="37" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>916</v>
       </c>
@@ -4852,7 +4865,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:43">
+    <row r="38" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>915</v>
       </c>
@@ -4944,7 +4957,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:43">
+    <row r="39" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>914</v>
       </c>
@@ -5036,13 +5049,13 @@
         <v>192</v>
       </c>
     </row>
-    <row r="40" spans="1:43"/>
-    <row r="41" spans="1:43" s="3" customFormat="1">
+    <row r="40" spans="1:43" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="42" spans="1:43">
+    <row r="42" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>916</v>
       </c>
@@ -5173,7 +5186,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:43">
+    <row r="43" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>915</v>
       </c>
@@ -5304,7 +5317,7 @@
         <v>-12</v>
       </c>
     </row>
-    <row r="44" spans="1:43">
+    <row r="44" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>914</v>
       </c>
@@ -5435,13 +5448,13 @@
         <v>228</v>
       </c>
     </row>
-    <row r="45" spans="1:43"/>
-    <row r="46" spans="1:43" s="3" customFormat="1">
+    <row r="45" spans="1:43" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="47" spans="1:43">
+    <row r="47" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>916</v>
       </c>
@@ -5461,7 +5474,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:43">
+    <row r="48" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>914</v>
       </c>
@@ -5481,13 +5494,13 @@
         <v>234</v>
       </c>
     </row>
-    <row r="49" spans="1:39"/>
-    <row r="50" spans="1:39" s="3" customFormat="1">
+    <row r="49" spans="1:39" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:39" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="51" spans="1:39">
+    <row r="51" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>916</v>
       </c>
@@ -5606,7 +5619,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:39">
+    <row r="52" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>915</v>
       </c>
@@ -5725,7 +5738,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:39">
+    <row r="53" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>914</v>
       </c>
@@ -5844,13 +5857,13 @@
         <v>272</v>
       </c>
     </row>
-    <row r="54" spans="1:39"/>
-    <row r="55" spans="1:39" s="3" customFormat="1">
+    <row r="54" spans="1:39" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="1:39" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="56" spans="1:39">
+    <row r="56" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>916</v>
       </c>
@@ -5942,7 +5955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:39">
+    <row r="57" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>915</v>
       </c>
@@ -6034,7 +6047,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:39">
+    <row r="58" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>914</v>
       </c>
@@ -6126,13 +6139,13 @@
         <v>301</v>
       </c>
     </row>
-    <row r="59" spans="1:39"/>
-    <row r="60" spans="1:39" s="3" customFormat="1">
+    <row r="59" spans="1:39" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="1:39" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="61" spans="1:39">
+    <row r="61" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>916</v>
       </c>
@@ -6152,7 +6165,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:39">
+    <row r="62" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>914</v>
       </c>
@@ -6172,14 +6185,14 @@
         <v>307</v>
       </c>
     </row>
-    <row r="63" spans="1:39"/>
-    <row r="64" spans="1:39" s="3" customFormat="1">
+    <row r="63" spans="1:39" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="1:39" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>308</v>
       </c>
       <c r="B64" s="2"/>
     </row>
-    <row r="65" spans="1:43">
+    <row r="65" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>916</v>
       </c>
@@ -6310,7 +6323,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="66" spans="1:43">
+    <row r="66" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>915</v>
       </c>
@@ -6441,7 +6454,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="67" spans="1:43">
+    <row r="67" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>914</v>
       </c>
@@ -6572,13 +6585,13 @@
         <v>345</v>
       </c>
     </row>
-    <row r="68" spans="1:43"/>
-    <row r="69" spans="1:43" s="3" customFormat="1">
+    <row r="68" spans="1:43" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="70" spans="1:43">
+    <row r="70" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>916</v>
       </c>
@@ -6598,7 +6611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:43">
+    <row r="71" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>914</v>
       </c>
@@ -6618,13 +6631,13 @@
         <v>351</v>
       </c>
     </row>
-    <row r="72" spans="1:43"/>
-    <row r="73" spans="1:43" s="3" customFormat="1">
+    <row r="72" spans="1:43" x14ac:dyDescent="0.3"/>
+    <row r="73" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="74" spans="1:43">
+    <row r="74" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>916</v>
       </c>
@@ -6716,7 +6729,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="1:43">
+    <row r="75" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>915</v>
       </c>
@@ -6808,7 +6821,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="76" spans="1:43">
+    <row r="76" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>914</v>
       </c>
@@ -6900,13 +6913,13 @@
         <v>939</v>
       </c>
     </row>
-    <row r="77" spans="1:43"/>
-    <row r="78" spans="1:43" s="3" customFormat="1">
+    <row r="77" spans="1:43" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="79" spans="1:43">
+    <row r="79" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>916</v>
       </c>
@@ -7013,7 +7026,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:43">
+    <row r="80" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>915</v>
       </c>
@@ -7120,7 +7133,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="81" spans="1:44">
+    <row r="81" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>914</v>
       </c>
@@ -7227,13 +7240,13 @@
         <v>410</v>
       </c>
     </row>
-    <row r="82" spans="1:44"/>
-    <row r="83" spans="1:44" s="3" customFormat="1">
+    <row r="82" spans="1:44" x14ac:dyDescent="0.3"/>
+    <row r="83" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="84" spans="1:44">
+    <row r="84" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>916</v>
       </c>
@@ -7367,7 +7380,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="85" spans="1:44">
+    <row r="85" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>915</v>
       </c>
@@ -7501,7 +7514,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:44">
+    <row r="86" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>914</v>
       </c>
@@ -7635,13 +7648,13 @@
         <v>452</v>
       </c>
     </row>
-    <row r="87" spans="1:44"/>
-    <row r="88" spans="1:44" s="3" customFormat="1">
+    <row r="87" spans="1:44" x14ac:dyDescent="0.3"/>
+    <row r="88" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="89" spans="1:44">
+    <row r="89" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>916</v>
       </c>
@@ -7658,7 +7671,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:44">
+    <row r="90" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>914</v>
       </c>
@@ -7675,13 +7688,13 @@
         <v>457</v>
       </c>
     </row>
-    <row r="91" spans="1:44"/>
-    <row r="92" spans="1:44" s="3" customFormat="1">
+    <row r="91" spans="1:44" x14ac:dyDescent="0.3"/>
+    <row r="92" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="93" spans="1:44">
+    <row r="93" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>916</v>
       </c>
@@ -7806,7 +7819,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="94" spans="1:44">
+    <row r="94" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>915</v>
       </c>
@@ -7931,7 +7944,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="95" spans="1:44">
+    <row r="95" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>914</v>
       </c>
@@ -8056,13 +8069,13 @@
         <v>498</v>
       </c>
     </row>
-    <row r="96" spans="1:44"/>
-    <row r="97" spans="1:40" s="3" customFormat="1">
+    <row r="96" spans="1:44" x14ac:dyDescent="0.3"/>
+    <row r="97" spans="1:40" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="98" spans="1:40">
+    <row r="98" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>916</v>
       </c>
@@ -8184,7 +8197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:40">
+    <row r="99" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>915</v>
       </c>
@@ -8306,7 +8319,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="100" spans="1:40">
+    <row r="100" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>914</v>
       </c>
@@ -8428,13 +8441,13 @@
         <v>538</v>
       </c>
     </row>
-    <row r="101" spans="1:40"/>
-    <row r="102" spans="1:40" s="3" customFormat="1">
+    <row r="101" spans="1:40" x14ac:dyDescent="0.3"/>
+    <row r="102" spans="1:40" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="103" spans="1:40">
+    <row r="103" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>916</v>
       </c>
@@ -8454,7 +8467,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="104" spans="1:40">
+    <row r="104" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>914</v>
       </c>
@@ -8474,8 +8487,8 @@
         <v>544</v>
       </c>
     </row>
-    <row r="105" spans="1:40"/>
-    <row r="106" spans="1:40" s="3" customFormat="1">
+    <row r="105" spans="1:40" x14ac:dyDescent="0.3"/>
+    <row r="106" spans="1:40" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>545</v>
       </c>
@@ -8483,7 +8496,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="107" spans="1:40">
+    <row r="107" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>916</v>
       </c>
@@ -8560,7 +8573,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="108" spans="1:40">
+    <row r="108" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>915</v>
       </c>
@@ -8637,7 +8650,7 @@
         <v>-12</v>
       </c>
     </row>
-    <row r="109" spans="1:40">
+    <row r="109" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>914</v>
       </c>
@@ -8714,13 +8727,13 @@
         <v>568</v>
       </c>
     </row>
-    <row r="110" spans="1:40"/>
-    <row r="111" spans="1:40" s="3" customFormat="1">
+    <row r="110" spans="1:40" x14ac:dyDescent="0.3"/>
+    <row r="111" spans="1:40" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="112" spans="1:40">
+    <row r="112" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
         <v>916</v>
       </c>
@@ -8806,7 +8819,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="113" spans="1:28">
+    <row r="113" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
         <v>915</v>
       </c>
@@ -8892,7 +8905,7 @@
         <v>-12</v>
       </c>
     </row>
-    <row r="114" spans="1:28" s="4" customFormat="1">
+    <row r="114" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
         <v>914</v>
       </c>
@@ -8978,13 +8991,13 @@
         <v>593</v>
       </c>
     </row>
-    <row r="115" spans="1:28"/>
-    <row r="116" spans="1:28" s="3" customFormat="1">
+    <row r="115" spans="1:28" x14ac:dyDescent="0.3"/>
+    <row r="116" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="117" spans="1:28">
+    <row r="117" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>916</v>
       </c>
@@ -9001,7 +9014,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:28">
+    <row r="118" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>914</v>
       </c>
@@ -9018,8 +9031,8 @@
         <v>598</v>
       </c>
     </row>
-    <row r="119" spans="1:28"/>
-    <row r="120" spans="1:28" s="3" customFormat="1">
+    <row r="119" spans="1:28" x14ac:dyDescent="0.3"/>
+    <row r="120" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>599</v>
       </c>
@@ -9027,7 +9040,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="121" spans="1:28">
+    <row r="121" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
         <v>916</v>
       </c>
@@ -9104,7 +9117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:28">
+    <row r="122" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
         <v>915</v>
       </c>
@@ -9181,7 +9194,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:28">
+    <row r="123" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
         <v>914</v>
       </c>
@@ -9258,13 +9271,13 @@
         <v>620</v>
       </c>
     </row>
-    <row r="124" spans="1:28"/>
-    <row r="125" spans="1:28" s="3" customFormat="1">
+    <row r="124" spans="1:28" x14ac:dyDescent="0.3"/>
+    <row r="125" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>621</v>
       </c>
     </row>
-    <row r="126" spans="1:28">
+    <row r="126" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>914</v>
       </c>
@@ -9299,13 +9312,13 @@
         <v>86</v>
       </c>
     </row>
-    <row r="127" spans="1:28"/>
-    <row r="128" spans="1:28" s="3" customFormat="1">
+    <row r="127" spans="1:28" x14ac:dyDescent="0.3"/>
+    <row r="128" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="129" spans="1:34">
+    <row r="129" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>916</v>
       </c>
@@ -9322,7 +9335,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="130" spans="1:34">
+    <row r="130" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>914</v>
       </c>
@@ -9339,13 +9352,13 @@
         <v>626</v>
       </c>
     </row>
-    <row r="131" spans="1:34"/>
-    <row r="132" spans="1:34" s="3" customFormat="1">
+    <row r="131" spans="1:34" x14ac:dyDescent="0.3"/>
+    <row r="132" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="133" spans="1:34">
+    <row r="133" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
         <v>916</v>
       </c>
@@ -9431,7 +9444,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="134" spans="1:34">
+    <row r="134" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
         <v>915</v>
       </c>
@@ -9517,7 +9530,7 @@
         <v>-12</v>
       </c>
     </row>
-    <row r="135" spans="1:34">
+    <row r="135" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
         <v>914</v>
       </c>
@@ -9603,13 +9616,13 @@
         <v>651</v>
       </c>
     </row>
-    <row r="136" spans="1:34"/>
-    <row r="137" spans="1:34" s="3" customFormat="1">
+    <row r="136" spans="1:34" x14ac:dyDescent="0.3"/>
+    <row r="137" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>652</v>
       </c>
     </row>
-    <row r="138" spans="1:34">
+    <row r="138" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
         <v>916</v>
       </c>
@@ -9701,7 +9714,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="139" spans="1:34">
+    <row r="139" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
         <v>915</v>
       </c>
@@ -9793,7 +9806,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="140" spans="1:34">
+    <row r="140" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
         <v>914</v>
       </c>
@@ -9885,13 +9898,13 @@
         <v>678</v>
       </c>
     </row>
-    <row r="141" spans="1:34"/>
-    <row r="142" spans="1:34" s="3" customFormat="1">
+    <row r="141" spans="1:34" x14ac:dyDescent="0.3"/>
+    <row r="142" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>679</v>
       </c>
     </row>
-    <row r="143" spans="1:34">
+    <row r="143" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
         <v>916</v>
       </c>
@@ -9995,7 +10008,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="144" spans="1:34">
+    <row r="144" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A144" s="5" t="s">
         <v>915</v>
       </c>
@@ -10099,7 +10112,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="145" spans="1:40">
+    <row r="145" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A145" s="5" t="s">
         <v>914</v>
       </c>
@@ -10203,13 +10216,13 @@
         <v>707</v>
       </c>
     </row>
-    <row r="146" spans="1:40"/>
-    <row r="147" spans="1:40" s="3" customFormat="1">
+    <row r="146" spans="1:40" x14ac:dyDescent="0.3"/>
+    <row r="147" spans="1:40" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="148" spans="1:40">
+    <row r="148" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>916</v>
       </c>
@@ -10226,7 +10239,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="1:40">
+    <row r="149" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>914</v>
       </c>
@@ -10243,13 +10256,13 @@
         <v>712</v>
       </c>
     </row>
-    <row r="150" spans="1:40"/>
-    <row r="151" spans="1:40" s="3" customFormat="1">
+    <row r="150" spans="1:40" x14ac:dyDescent="0.3"/>
+    <row r="151" spans="1:40" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>713</v>
       </c>
     </row>
-    <row r="152" spans="1:40">
+    <row r="152" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A152" s="5" t="s">
         <v>916</v>
       </c>
@@ -10368,7 +10381,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="153" spans="1:40">
+    <row r="153" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
         <v>915</v>
       </c>
@@ -10487,7 +10500,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="154" spans="1:40">
+    <row r="154" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
         <v>914</v>
       </c>
@@ -10606,13 +10619,13 @@
         <v>751</v>
       </c>
     </row>
-    <row r="155" spans="1:40"/>
-    <row r="156" spans="1:40" s="3" customFormat="1">
+    <row r="155" spans="1:40" x14ac:dyDescent="0.3"/>
+    <row r="156" spans="1:40" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>752</v>
       </c>
     </row>
-    <row r="157" spans="1:40">
+    <row r="157" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
         <v>916</v>
       </c>
@@ -10734,7 +10747,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="158" spans="1:40">
+    <row r="158" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A158" s="5" t="s">
         <v>915</v>
       </c>
@@ -10856,7 +10869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:40">
+    <row r="159" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A159" s="5" t="s">
         <v>914</v>
       </c>
@@ -10978,13 +10991,13 @@
         <v>791</v>
       </c>
     </row>
-    <row r="160" spans="1:40"/>
-    <row r="161" spans="1:37" s="3" customFormat="1">
+    <row r="160" spans="1:40" x14ac:dyDescent="0.3"/>
+    <row r="161" spans="1:37" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>792</v>
       </c>
     </row>
-    <row r="162" spans="1:37">
+    <row r="162" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>916</v>
       </c>
@@ -11004,7 +11017,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="163" spans="1:37">
+    <row r="163" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>914</v>
       </c>
@@ -11024,13 +11037,13 @@
         <v>797</v>
       </c>
     </row>
-    <row r="164" spans="1:37"/>
-    <row r="165" spans="1:37" s="3" customFormat="1">
+    <row r="164" spans="1:37" x14ac:dyDescent="0.3"/>
+    <row r="165" spans="1:37" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>798</v>
       </c>
     </row>
-    <row r="166" spans="1:37">
+    <row r="166" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A166" s="5" t="s">
         <v>916</v>
       </c>
@@ -11140,7 +11153,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="167" spans="1:37">
+    <row r="167" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
         <v>915</v>
       </c>
@@ -11250,7 +11263,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="168" spans="1:37">
+    <row r="168" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A168" s="5" t="s">
         <v>914</v>
       </c>
@@ -11360,13 +11373,13 @@
         <v>832</v>
       </c>
     </row>
-    <row r="169" spans="1:37"/>
-    <row r="170" spans="1:37" s="3" customFormat="1">
+    <row r="169" spans="1:37" x14ac:dyDescent="0.3"/>
+    <row r="170" spans="1:37" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>833</v>
       </c>
     </row>
-    <row r="171" spans="1:37">
+    <row r="171" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A171" s="5" t="s">
         <v>916</v>
       </c>
@@ -11479,7 +11492,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="172" spans="1:37">
+    <row r="172" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A172" s="5" t="s">
         <v>915</v>
       </c>
@@ -11592,7 +11605,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="173" spans="1:37">
+    <row r="173" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A173" s="5" t="s">
         <v>914</v>
       </c>
@@ -11705,13 +11718,13 @@
         <v>867</v>
       </c>
     </row>
-    <row r="174" spans="1:37"/>
-    <row r="175" spans="1:37" s="3" customFormat="1">
+    <row r="174" spans="1:37" x14ac:dyDescent="0.3"/>
+    <row r="175" spans="1:37" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
         <v>868</v>
       </c>
     </row>
-    <row r="176" spans="1:37">
+    <row r="176" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A176" s="5" t="s">
         <v>916</v>
       </c>
@@ -11776,7 +11789,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="177" spans="1:24">
+    <row r="177" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A177" s="5" t="s">
         <v>915</v>
       </c>
@@ -11841,7 +11854,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="178" spans="1:24">
+    <row r="178" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A178" s="5" t="s">
         <v>914</v>
       </c>
@@ -11906,13 +11919,13 @@
         <v>888</v>
       </c>
     </row>
-    <row r="179" spans="1:24"/>
-    <row r="180" spans="1:24" s="3" customFormat="1">
+    <row r="179" spans="1:24" x14ac:dyDescent="0.3"/>
+    <row r="180" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
         <v>889</v>
       </c>
     </row>
-    <row r="181" spans="1:24">
+    <row r="181" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A181" s="5" t="s">
         <v>916</v>
       </c>
@@ -11986,7 +11999,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="182" spans="1:24">
+    <row r="182" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A182" s="5" t="s">
         <v>915</v>
       </c>
@@ -12060,7 +12073,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="183" spans="1:24">
+    <row r="183" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A183" s="5" t="s">
         <v>914</v>
       </c>
@@ -12134,7 +12147,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="184" spans="1:24"/>
+    <row r="184" spans="1:24" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>